<commit_message>
feat: delete HBCDD from drafts and Data_analysis vignette and results
</commit_message>
<xml_diff>
--- a/inst/results/Data_analysis/4.test_dunn_alim.xlsx
+++ b/inst/results/Data_analysis/4.test_dunn_alim.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -373,11 +373,6 @@
           <t>PFAS</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>HBCDD</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -391,9 +386,6 @@
       <c r="C2">
         <v>0.1188</v>
       </c>
-      <c r="D2">
-        <v>2.527E-05</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -407,9 +399,6 @@
       <c r="C3">
         <v>0.01035</v>
       </c>
-      <c r="D3">
-        <v>0.5179</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -422,9 +411,6 @@
       </c>
       <c r="C4">
         <v>3.121E-05</v>
-      </c>
-      <c r="D4">
-        <v>8.278E-07</v>
       </c>
     </row>
   </sheetData>

</xml_diff>